<commit_message>
Fix special breaches having the wrong mage prefix
</commit_message>
<xml_diff>
--- a/Breaches.xlsx
+++ b/Breaches.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Lexive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{533E991B-248D-4217-99E3-367E263FDE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54C84EA-E6C3-4242-83E0-8C413C5ACE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DCE14C3E-305F-4967-A27E-679FF7EFD469}"/>
   </bookViews>
@@ -24,6 +24,13 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -111,9 +118,6 @@
     <t>Up to 10 Surge tokens can be placed on the Ancient Breach. When a spell is cast from this breach, that spell deals 1 additional damage for each Surge token placed on that breach.</t>
   </si>
   <si>
-    <t>Gygar</t>
-  </si>
-  <si>
     <t>Defender Breach</t>
   </si>
   <si>
@@ -129,18 +133,12 @@
     <t>Once Opened: On Cast: Gain 1 charge.</t>
   </si>
   <si>
-    <t>Mazra</t>
-  </si>
-  <si>
     <t>Forged Breach</t>
   </si>
   <si>
     <t>When you open this, gain a card that costs 4$ or less from any supply pile.</t>
   </si>
   <si>
-    <t>Thraxir</t>
-  </si>
-  <si>
     <t>Honed Breach</t>
   </si>
   <si>
@@ -208,6 +206,15 @@
   </si>
   <si>
     <t>Reth</t>
+  </si>
+  <si>
+    <t>Gygar (NA)</t>
+  </si>
+  <si>
+    <t>Mazra (NA)</t>
+  </si>
+  <si>
+    <t>Thraxir (O)</t>
   </si>
 </sst>
 </file>
@@ -640,7 +647,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +690,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -691,10 +698,10 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -717,10 +724,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -743,10 +750,10 @@
         <v>5</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -772,7 +779,7 @@
         <v>11</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -798,12 +805,12 @@
         <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -811,10 +818,10 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -918,12 +925,12 @@
         <v>23</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
         <v>4</v>
@@ -941,15 +948,15 @@
         <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1">
         <v>3</v>
@@ -967,15 +974,15 @@
         <v>9</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -983,15 +990,15 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -1009,15 +1016,15 @@
         <v>4</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>2</v>
@@ -1035,15 +1042,15 @@
         <v>5</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>
@@ -1061,15 +1068,15 @@
         <v>9</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1">
         <v>4</v>
@@ -1087,15 +1094,15 @@
         <v>13</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1103,15 +1110,15 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1">
         <v>4</v>
@@ -1129,15 +1136,15 @@
         <v>13</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B21" s="1">
         <v>4</v>
@@ -1155,15 +1162,15 @@
         <v>13</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1171,15 +1178,15 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B23" s="1">
         <v>2</v>
@@ -1197,15 +1204,15 @@
         <v>0</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1">
         <v>3</v>
@@ -1223,15 +1230,15 @@
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1">
         <v>4</v>
@@ -1249,26 +1256,26 @@
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -1286,10 +1293,10 @@
         <v>9</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>